<commit_message>
Small fix in the data_table
- Removed whitespace at the end of the Genre: "Contribution to Collected
Edition"
</commit_message>
<xml_diff>
--- a/res/data_table.xlsx
+++ b/res/data_table.xlsx
@@ -1463,9 +1463,6 @@
     <t>Book Chapter</t>
   </si>
   <si>
-    <t xml:space="preserve">Contribution to Collected Edition </t>
-  </si>
-  <si>
     <t>Contribution to Commentary</t>
   </si>
   <si>
@@ -1644,6 +1641,9 @@
   </si>
   <si>
     <t>por - Portuguese</t>
+  </si>
+  <si>
+    <t>Contribution to Collected Edition</t>
   </si>
 </sst>
 </file>
@@ -2057,8 +2057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,16 +2106,16 @@
         <v>432</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>436</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2142,10 +2142,10 @@
         <v>415</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>437</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>438</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>418</v>
@@ -2154,10 +2154,10 @@
         <v>411</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>440</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>423</v>
@@ -2172,16 +2172,16 @@
         <v>426</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>444</v>
       </c>
       <c r="Q3" s="1" t="s">
         <v>422</v>
@@ -2231,10 +2231,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>445</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>446</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2265,19 +2265,19 @@
         <v>416</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>450</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="1"/>
@@ -2301,70 +2301,70 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -2372,70 +2372,70 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -3544,7 +3544,7 @@
         <v>92</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>93</v>
@@ -3974,22 +3974,22 @@
         <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -4013,22 +4013,22 @@
         <v>134</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>483</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>484</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -4052,19 +4052,19 @@
         <v>135</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>461</v>
-      </c>
       <c r="F36" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -4092,16 +4092,16 @@
         <v>137</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -4126,19 +4126,19 @@
         <v>138</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -4166,16 +4166,16 @@
         <v>140</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -4203,16 +4203,16 @@
         <v>140</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -4237,19 +4237,19 @@
         <v>142</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -4526,7 +4526,7 @@
         <v>411</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N47" s="5" t="s">
         <v>412</v>
@@ -5478,7 +5478,7 @@
         <v>411</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N71" s="5" t="s">
         <v>412</v>
@@ -5953,7 +5953,7 @@
         <v>411</v>
       </c>
       <c r="M80" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N80" s="5" t="s">
         <v>412</v>

</xml_diff>

<commit_message>
Removed 'eSciDoc' as value of the 'Identifier'-fields from the data_tabl
- Removed the test data value 'eSciDoc' from the test data types:
'identifier create item', 'identifier source' and 'identifier source
create item' in the data_tabl.xlsx
</commit_message>
<xml_diff>
--- a/res/data_table.xlsx
+++ b/res/data_table.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="135" windowWidth="20115" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19395" windowHeight="8250"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="493">
   <si>
     <t>SOURCE_DEP</t>
   </si>
@@ -1380,9 +1381,6 @@
   </si>
   <si>
     <t>eDoc</t>
-  </si>
-  <si>
-    <t>eSciDoc</t>
   </si>
   <si>
     <t>Other</t>
@@ -2060,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="G78" sqref="G78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2071,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>425</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2104,19 +2102,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>430</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>431</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -2140,58 +2138,58 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>439</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="1"/>
@@ -2203,10 +2201,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2234,10 +2232,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>440</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>441</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2265,22 +2263,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>445</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="1"/>
@@ -2304,70 +2302,70 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -2375,70 +2373,70 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -2446,70 +2444,70 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="192" x14ac:dyDescent="0.25">
@@ -3547,7 +3545,7 @@
         <v>92</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>93</v>
@@ -3650,13 +3648,13 @@
         <v>99</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>100</v>
@@ -3665,13 +3663,13 @@
         <v>101</v>
       </c>
       <c r="G29" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>100</v>
@@ -3680,13 +3678,13 @@
         <v>101</v>
       </c>
       <c r="L29" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="M29" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>100</v>
@@ -3695,13 +3693,13 @@
         <v>101</v>
       </c>
       <c r="Q29" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="R29" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="R29" s="1" t="s">
+      <c r="S29" s="1" t="s">
         <v>492</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>493</v>
       </c>
       <c r="T29" s="1" t="s">
         <v>100</v>
@@ -3710,10 +3708,10 @@
         <v>101</v>
       </c>
       <c r="V29" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="W29" s="1" t="s">
         <v>491</v>
-      </c>
-      <c r="W29" s="1" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="48" x14ac:dyDescent="0.25">
@@ -3977,22 +3975,22 @@
         <v>130</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>487</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>488</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -4016,22 +4014,22 @@
         <v>131</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>479</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -4055,19 +4053,19 @@
         <v>132</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>456</v>
-      </c>
       <c r="F36" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -4095,16 +4093,16 @@
         <v>134</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -4129,19 +4127,19 @@
         <v>135</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -4169,16 +4167,16 @@
         <v>137</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -4206,16 +4204,16 @@
         <v>137</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -4240,19 +4238,19 @@
         <v>139</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -4513,9 +4511,7 @@
       <c r="G47" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="H47" s="5" t="s">
-        <v>406</v>
-      </c>
+      <c r="H47" s="5"/>
       <c r="I47" s="5" t="s">
         <v>171</v>
       </c>
@@ -4526,16 +4522,16 @@
         <v>173</v>
       </c>
       <c r="L47" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="M47" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="N47" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="M47" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="N47" s="5" t="s">
+      <c r="O47" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="O47" s="5" t="s">
-        <v>409</v>
       </c>
       <c r="P47" s="5" t="s">
         <v>174</v>
@@ -4547,7 +4543,7 @@
         <v>176</v>
       </c>
       <c r="S47" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="T47" s="5" t="s">
         <v>177</v>
@@ -4671,7 +4667,7 @@
         <v>207</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>208</v>
@@ -5326,40 +5322,40 @@
         <v>292</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="D69" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="E69" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="E69" s="5" t="s">
+      <c r="F69" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="F69" s="5" t="s">
+      <c r="G69" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="G69" s="5" t="s">
+      <c r="H69" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="H69" s="5" t="s">
+      <c r="I69" s="5" t="s">
         <v>417</v>
       </c>
-      <c r="I69" s="5" t="s">
+      <c r="J69" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="J69" s="5" t="s">
+      <c r="K69" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="K69" s="5" t="s">
+      <c r="L69" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="L69" s="5" t="s">
+      <c r="M69" s="5" t="s">
         <v>421</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>422</v>
       </c>
       <c r="N69" s="5"/>
       <c r="O69" s="5"/>
@@ -5465,9 +5461,7 @@
       <c r="G71" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="H71" s="5" t="s">
-        <v>406</v>
-      </c>
+      <c r="H71" s="5"/>
       <c r="I71" s="5" t="s">
         <v>171</v>
       </c>
@@ -5478,16 +5472,16 @@
         <v>173</v>
       </c>
       <c r="L71" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="M71" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="N71" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="M71" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="N71" s="5" t="s">
+      <c r="O71" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="O71" s="5" t="s">
-        <v>409</v>
       </c>
       <c r="P71" s="5" t="s">
         <v>174</v>
@@ -5499,7 +5493,7 @@
         <v>176</v>
       </c>
       <c r="S71" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="T71" s="5" t="s">
         <v>177</v>
@@ -5940,9 +5934,7 @@
       <c r="G80" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="H80" s="5" t="s">
-        <v>406</v>
-      </c>
+      <c r="H80" s="5"/>
       <c r="I80" s="5" t="s">
         <v>171</v>
       </c>
@@ -5953,16 +5945,16 @@
         <v>173</v>
       </c>
       <c r="L80" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="M80" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="N80" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="M80" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="N80" s="5" t="s">
+      <c r="O80" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="O80" s="5" t="s">
-        <v>409</v>
       </c>
       <c r="P80" s="5" t="s">
         <v>174</v>
@@ -5974,7 +5966,7 @@
         <v>176</v>
       </c>
       <c r="S80" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="T80" s="5" t="s">
         <v>177</v>

</xml_diff>